<commit_message>
updated with records through Oct 20
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears.xlsx
+++ b/output/natl_grandtots_bothyears.xlsx
@@ -407,22 +407,22 @@
         <v>12997090</v>
       </c>
       <c r="C2">
-        <v>49314696</v>
+        <v>50522576</v>
       </c>
       <c r="D2">
-        <v>24103846</v>
+        <v>26543024</v>
       </c>
       <c r="E2">
-        <v>15067054</v>
+        <v>16274934</v>
       </c>
       <c r="F2">
-        <v>43.99</v>
+        <v>47.52</v>
       </c>
       <c r="G2">
-        <v>11106756</v>
+        <v>13545934</v>
       </c>
       <c r="H2">
-        <v>85.45999999999999</v>
+        <v>104.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for 13 days before election
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears.xlsx
+++ b/output/natl_grandtots_bothyears.xlsx
@@ -401,28 +401,28 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>34247642</v>
+        <v>36204183</v>
       </c>
       <c r="B2">
-        <v>12997090</v>
+        <v>16015905</v>
       </c>
       <c r="C2">
-        <v>50522576</v>
+        <v>50522577</v>
       </c>
       <c r="D2">
         <v>26543024</v>
       </c>
       <c r="E2">
-        <v>16274934</v>
+        <v>14318394</v>
       </c>
       <c r="F2">
-        <v>47.52</v>
+        <v>39.55</v>
       </c>
       <c r="G2">
-        <v>13545934</v>
+        <v>10527119</v>
       </c>
       <c r="H2">
-        <v>104.22</v>
+        <v>65.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data from 12 days before election
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears.xlsx
+++ b/output/natl_grandtots_bothyears.xlsx
@@ -401,28 +401,28 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>36204183</v>
+        <v>38194725</v>
       </c>
       <c r="B2">
-        <v>16015905</v>
+        <v>18852567</v>
       </c>
       <c r="C2">
-        <v>50522577</v>
+        <v>54607854</v>
       </c>
       <c r="D2">
-        <v>26543024</v>
+        <v>31865985</v>
       </c>
       <c r="E2">
-        <v>14318394</v>
+        <v>16413129</v>
       </c>
       <c r="F2">
-        <v>39.55</v>
+        <v>42.97</v>
       </c>
       <c r="G2">
-        <v>10527119</v>
+        <v>13013418</v>
       </c>
       <c r="H2">
-        <v>65.73</v>
+        <v>69.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>